<commit_message>
fixed the wrong dates & changed Mirsalari with Bazgir in first week
</commit_message>
<xml_diff>
--- a/03 - Khordad.xlsx
+++ b/03 - Khordad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\MaktabSharif\Works\Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB7F869-9060-4FB5-A85A-F9778E9DC2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773AE827-FC55-4885-B493-6C92330DBB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF2BF689-5E91-4292-9B13-39FB55D30CFD}"/>
   </bookViews>
@@ -183,9 +183,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -196,6 +193,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +515,7 @@
   <dimension ref="E3:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,28 +536,28 @@
       </c>
     </row>
     <row r="5" spans="5:20" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="P5" s="2" t="s">
@@ -577,163 +577,163 @@
       </c>
     </row>
     <row r="6" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="7">
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="6">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8</v>
+      </c>
+      <c r="J8" s="2">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2">
         <v>6</v>
       </c>
-      <c r="F6" s="7">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>4</v>
-      </c>
-      <c r="H6" s="7">
-        <v>3</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="8" t="s">
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="6">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6">
+        <v>18</v>
+      </c>
+      <c r="G10" s="2">
+        <v>17</v>
+      </c>
+      <c r="H10" s="6">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2">
+        <v>15</v>
+      </c>
+      <c r="J10" s="2">
+        <v>14</v>
+      </c>
+      <c r="K10" s="2">
+        <v>13</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="6">
+        <v>26</v>
+      </c>
+      <c r="F12" s="6">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2">
+        <v>24</v>
+      </c>
+      <c r="H12" s="6">
+        <v>23</v>
+      </c>
+      <c r="I12" s="2">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2">
+        <v>20</v>
+      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="7">
-        <v>13</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="H13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2">
-        <v>11</v>
-      </c>
-      <c r="H8" s="7">
-        <v>10</v>
-      </c>
-      <c r="I8" s="2">
-        <v>9</v>
-      </c>
-      <c r="J8" s="2">
-        <v>8</v>
-      </c>
-      <c r="K8" s="2">
-        <v>7</v>
-      </c>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="7">
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>31</v>
+      </c>
+      <c r="H14" s="6">
+        <v>30</v>
+      </c>
+      <c r="I14" s="2">
         <v>20</v>
       </c>
-      <c r="F10" s="7">
-        <v>19</v>
-      </c>
-      <c r="G10" s="2">
-        <v>18</v>
-      </c>
-      <c r="H10" s="7">
-        <v>17</v>
-      </c>
-      <c r="I10" s="2">
-        <v>16</v>
-      </c>
-      <c r="J10" s="2">
-        <v>15</v>
-      </c>
-      <c r="K10" s="2">
-        <v>14</v>
-      </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="7">
+      <c r="J14" s="2">
+        <v>28</v>
+      </c>
+      <c r="K14" s="2">
         <v>27</v>
       </c>
-      <c r="F12" s="7">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2">
-        <v>25</v>
-      </c>
-      <c r="H12" s="7">
-        <v>24</v>
-      </c>
-      <c r="I12" s="2">
-        <v>23</v>
-      </c>
-      <c r="J12" s="2">
-        <v>22</v>
-      </c>
-      <c r="K12" s="2">
-        <v>21</v>
-      </c>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="5:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="7">
-        <v>31</v>
-      </c>
-      <c r="I14" s="2">
-        <v>30</v>
-      </c>
-      <c r="J14" s="2">
-        <v>29</v>
-      </c>
-      <c r="K14" s="2">
-        <v>28</v>
-      </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="5:20" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -747,19 +747,19 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M17" s="4"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M18" s="4"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M19" s="4"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M20" s="4"/>
+      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M21" s="4"/>
+      <c r="M21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>